<commit_message>
Add first after work walk of the year.
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27211"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marks/projects/walk/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="987"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="15480" tabRatio="987"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="1" r:id="rId1"/>
@@ -17,11 +12,8 @@
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="145621" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -288,40 +280,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>31.0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>87.0</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>180.0</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>300.0</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>455.0</c:v>
+                  <c:v>455</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>635.0</c:v>
+                  <c:v>635</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>821.0</c:v>
+                  <c:v>821</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>976.0</c:v>
+                  <c:v>976</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1096.0</c:v>
+                  <c:v>1096</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1189.0</c:v>
+                  <c:v>1189</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1249.0</c:v>
+                  <c:v>1249</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1280.0</c:v>
+                  <c:v>1280</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -415,10 +407,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>25.0</c:v>
+                  <c:v>26.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.0</c:v>
+                  <c:v>26.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -440,12 +432,13 @@
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2136680160"/>
-        <c:axId val="2136683376"/>
+        <c:axId val="80794752"/>
+        <c:axId val="80796288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2136680160"/>
+        <c:axId val="80794752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -483,7 +476,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2136683376"/>
+        <c:crossAx val="80796288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -491,7 +484,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2136683376"/>
+        <c:axId val="80796288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -539,7 +532,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2136680160"/>
+        <c:crossAx val="80794752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -873,7 +866,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -888,7 +881,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -904,9 +897,9 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -926,13 +919,13 @@
       </c>
       <c r="F1">
         <f>G1</f>
-        <v>25</v>
+        <v>26.5</v>
       </c>
       <c r="G1">
-        <v>25</v>
+        <v>26.5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -952,10 +945,10 @@
       </c>
       <c r="F2">
         <f>F1+G2</f>
-        <v>25</v>
+        <v>26.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -974,7 +967,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -993,7 +986,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1012,7 +1005,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1031,7 +1024,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1050,7 +1043,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1069,7 +1062,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1088,7 +1081,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1107,7 +1100,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1126,7 +1119,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1157,7 +1150,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1170,7 +1163,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Add walk to spreadsheet
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -1,20 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27211"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marks/projects/walk/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="987" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Chart1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Chart1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -25,77 +35,53 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t xml:space="preserve">January</t>
+    <t>January</t>
   </si>
   <si>
-    <t xml:space="preserve">February</t>
+    <t>February</t>
   </si>
   <si>
-    <t xml:space="preserve">March</t>
+    <t>March</t>
   </si>
   <si>
-    <t xml:space="preserve">April</t>
+    <t>April</t>
   </si>
   <si>
-    <t xml:space="preserve">May</t>
+    <t>May</t>
   </si>
   <si>
-    <t xml:space="preserve">June</t>
+    <t>June</t>
   </si>
   <si>
-    <t xml:space="preserve">July</t>
+    <t>July</t>
   </si>
   <si>
-    <t xml:space="preserve">August</t>
+    <t>August</t>
   </si>
   <si>
-    <t xml:space="preserve">September</t>
+    <t>September</t>
   </si>
   <si>
-    <t xml:space="preserve">October</t>
+    <t>October</t>
   </si>
   <si>
-    <t xml:space="preserve">November</t>
+    <t>November</t>
   </si>
   <si>
-    <t xml:space="preserve">December</t>
+    <t>December</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -107,7 +93,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -115,45 +101,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -212,29 +170,44 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
+  <c:style val="18"/>
   <c:chart>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4a7ebb"/>
-            </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="4a7ebb"/>
+                <a:srgbClr val="4A7EBB"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -243,13 +216,26 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -302,40 +288,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>31</c:v>
+                  <c:v>31.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>87</c:v>
+                  <c:v>87.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>180</c:v>
+                  <c:v>180.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>300</c:v>
+                  <c:v>300.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>455</c:v>
+                  <c:v>455.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>635</c:v>
+                  <c:v>635.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>821</c:v>
+                  <c:v>821.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>976</c:v>
+                  <c:v>976.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1096</c:v>
+                  <c:v>1096.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1189</c:v>
+                  <c:v>1189.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1249</c:v>
+                  <c:v>1249.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1280</c:v>
+                  <c:v>1280.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -346,12 +332,9 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="be4b48"/>
-            </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="be4b48"/>
+                <a:srgbClr val="BE4B48"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -360,13 +343,26 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -419,46 +415,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>34.5</c:v>
+                  <c:v>37.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v/>
+                  <c:v>37.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
             <a:ln>
@@ -466,12 +440,12 @@
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="39962255"/>
-        <c:axId val="87889"/>
+        <c:smooth val="0"/>
+        <c:axId val="2143769888"/>
+        <c:axId val="2143766656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39962255"/>
+        <c:axId val="2143769888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -491,30 +465,33 @@
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:uFill>
                   <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a:uFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87889"/>
+        <c:crossAx val="2143766656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87889"/>
+        <c:axId val="2143766656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -544,29 +521,31 @@
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:uFill>
                   <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a:uFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39962255"/>
+        <c:crossAx val="2143769888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -575,6 +554,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -585,20 +565,26 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln>
       <a:noFill/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -612,14 +598,14 @@
       <xdr:row>37</xdr:row>
       <xdr:rowOff>64080</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
-        <a:ext cx="9644400" cy="7112520"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -632,347 +618,563 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="true"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+    <sheetView topLeftCell="A17" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="65" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O5" activeCellId="0" sqref="O5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="n">
+      <c r="B1">
         <v>31</v>
       </c>
-      <c r="C1" s="0" t="n">
+      <c r="C1">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="n">
-        <f aca="false">B1*C1</f>
+      <c r="D1">
+        <f t="shared" ref="D1:D12" si="0">B1*C1</f>
         <v>31</v>
       </c>
-      <c r="E1" s="0" t="n">
-        <f aca="false">D1</f>
+      <c r="E1">
+        <f>D1</f>
         <v>31</v>
       </c>
-      <c r="F1" s="0" t="n">
-        <f aca="false">G1</f>
-        <v>34.5</v>
-      </c>
-      <c r="G1" s="0" t="n">
-        <v>34.5</v>
+      <c r="F1">
+        <f>G1</f>
+        <v>37</v>
+      </c>
+      <c r="G1">
+        <v>37</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2">
         <v>28</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2">
         <v>2</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <f aca="false">B2*C2</f>
+      <c r="D2">
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <f aca="false">D2+E1</f>
+      <c r="E2">
+        <f t="shared" ref="E2:E12" si="1">D2+E1</f>
         <v>87</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <f aca="false">F1+G2</f>
-        <v>34.5</v>
+      <c r="F2">
+        <f>F1+G2</f>
+        <v>37</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3">
         <v>31</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3">
         <v>3</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <f aca="false">B3*C3</f>
+      <c r="D3">
+        <f t="shared" si="0"/>
         <v>93</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <f aca="false">D3+E2</f>
+      <c r="E3">
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4">
         <v>30</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4">
         <v>4</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <f aca="false">B4*C4</f>
+      <c r="D4">
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="E4" s="0" t="n">
-        <f aca="false">D4+E3</f>
+      <c r="E4">
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5">
         <v>31</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5">
         <v>5</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <f aca="false">B5*C5</f>
+      <c r="D5">
+        <f t="shared" si="0"/>
         <v>155</v>
       </c>
-      <c r="E5" s="0" t="n">
-        <f aca="false">D5+E4</f>
+      <c r="E5">
+        <f t="shared" si="1"/>
         <v>455</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6">
         <v>30</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6">
         <v>6</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <f aca="false">B6*C6</f>
+      <c r="D6">
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
-      <c r="E6" s="0" t="n">
-        <f aca="false">D6+E5</f>
+      <c r="E6">
+        <f t="shared" si="1"/>
         <v>635</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7">
         <v>31</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7">
         <v>6</v>
       </c>
-      <c r="D7" s="0" t="n">
-        <f aca="false">B7*C7</f>
+      <c r="D7">
+        <f t="shared" si="0"/>
         <v>186</v>
       </c>
-      <c r="E7" s="0" t="n">
-        <f aca="false">D7+E6</f>
+      <c r="E7">
+        <f t="shared" si="1"/>
         <v>821</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8">
         <v>31</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8">
         <v>5</v>
       </c>
-      <c r="D8" s="0" t="n">
-        <f aca="false">B8*C8</f>
+      <c r="D8">
+        <f t="shared" si="0"/>
         <v>155</v>
       </c>
-      <c r="E8" s="0" t="n">
-        <f aca="false">D8+E7</f>
+      <c r="E8">
+        <f t="shared" si="1"/>
         <v>976</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9">
         <v>30</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9">
         <v>4</v>
       </c>
-      <c r="D9" s="0" t="n">
-        <f aca="false">B9*C9</f>
+      <c r="D9">
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="E9" s="0" t="n">
-        <f aca="false">D9+E8</f>
+      <c r="E9">
+        <f t="shared" si="1"/>
         <v>1096</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10">
         <v>31</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10">
         <v>3</v>
       </c>
-      <c r="D10" s="0" t="n">
-        <f aca="false">B10*C10</f>
+      <c r="D10">
+        <f t="shared" si="0"/>
         <v>93</v>
       </c>
-      <c r="E10" s="0" t="n">
-        <f aca="false">D10+E9</f>
+      <c r="E10">
+        <f t="shared" si="1"/>
         <v>1189</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11">
         <v>30</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11" s="0" t="n">
-        <f aca="false">B11*C11</f>
+      <c r="D11">
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="E11" s="0" t="n">
-        <f aca="false">D11+E10</f>
+      <c r="E11">
+        <f t="shared" si="1"/>
         <v>1249</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12">
         <v>31</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12" s="0" t="n">
-        <f aca="false">B12*C12</f>
+      <c r="D12">
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="E12" s="0" t="n">
-        <f aca="false">D12+E11</f>
+      <c r="E12">
+        <f t="shared" si="1"/>
         <v>1280</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="65" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="65" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add walk from Euston to Holborn
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -1,19 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987"/>
   </bookViews>
   <sheets>
-    <sheet name="Chart1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Chart1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,82 +24,53 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t xml:space="preserve">January</t>
+    <t>January</t>
   </si>
   <si>
-    <t xml:space="preserve">February</t>
+    <t>February</t>
   </si>
   <si>
-    <t xml:space="preserve">March</t>
+    <t>March</t>
   </si>
   <si>
-    <t xml:space="preserve">April</t>
+    <t>April</t>
   </si>
   <si>
-    <t xml:space="preserve">May</t>
+    <t>May</t>
   </si>
   <si>
-    <t xml:space="preserve">June</t>
+    <t>June</t>
   </si>
   <si>
-    <t xml:space="preserve">July</t>
+    <t>July</t>
   </si>
   <si>
-    <t xml:space="preserve">August</t>
+    <t>August</t>
   </si>
   <si>
-    <t xml:space="preserve">September</t>
+    <t>September</t>
   </si>
   <si>
-    <t xml:space="preserve">October</t>
+    <t>October</t>
   </si>
   <si>
-    <t xml:space="preserve">November</t>
+    <t>November</t>
   </si>
   <si>
-    <t xml:space="preserve">December</t>
+    <t>December</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -112,7 +82,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -120,45 +90,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -217,29 +159,44 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4a7ebb"/>
-            </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="4a7ebb"/>
+                <a:srgbClr val="4A7EBB"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -254,6 +211,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -351,12 +309,9 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="be4b48"/>
-            </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="be4b48"/>
+                <a:srgbClr val="BE4B48"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -371,6 +326,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -424,46 +380,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>40.5</c:v>
+                  <c:v>41.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v/>
+                  <c:v>41.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
             <a:ln>
@@ -471,12 +405,13 @@
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="74552855"/>
-        <c:axId val="28216234"/>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="69343488"/>
+        <c:axId val="69349376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74552855"/>
+        <c:axId val="69343488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -496,30 +431,33 @@
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:uFill>
                   <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a:uFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28216234"/>
+        <c:crossAx val="69349376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="28216234"/>
+        <c:axId val="69349376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -549,29 +487,31 @@
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:uFill>
                   <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a:uFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74552855"/>
+        <c:crossAx val="69343488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -580,6 +520,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -590,20 +531,26 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln>
       <a:noFill/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -617,14 +564,14 @@
       <xdr:row>37</xdr:row>
       <xdr:rowOff>63360</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
-        <a:ext cx="9643680" cy="7111800"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -637,347 +584,599 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="true"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="n">
+      <c r="B1">
         <v>31</v>
       </c>
-      <c r="C1" s="0" t="n">
+      <c r="C1">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="n">
-        <f aca="false">B1*C1</f>
+      <c r="D1">
+        <f t="shared" ref="D1:D12" si="0">B1*C1</f>
         <v>31</v>
       </c>
-      <c r="E1" s="0" t="n">
-        <f aca="false">D1</f>
+      <c r="E1">
+        <f>D1</f>
         <v>31</v>
       </c>
-      <c r="F1" s="0" t="n">
-        <f aca="false">G1</f>
-        <v>40.5</v>
-      </c>
-      <c r="G1" s="0" t="n">
-        <v>40.5</v>
+      <c r="F1">
+        <f>G1</f>
+        <v>41.5</v>
+      </c>
+      <c r="G1">
+        <v>41.5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2">
         <v>28</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2">
         <v>2</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <f aca="false">B2*C2</f>
+      <c r="D2">
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <f aca="false">D2+E1</f>
+      <c r="E2">
+        <f t="shared" ref="E2:E12" si="1">D2+E1</f>
         <v>87</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <f aca="false">F1+G2</f>
-        <v>40.5</v>
+      <c r="F2">
+        <f>F1+G2</f>
+        <v>41.5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3">
         <v>31</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3">
         <v>3</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <f aca="false">B3*C3</f>
+      <c r="D3">
+        <f t="shared" si="0"/>
         <v>93</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <f aca="false">D3+E2</f>
+      <c r="E3">
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4">
         <v>30</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4">
         <v>4</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <f aca="false">B4*C4</f>
+      <c r="D4">
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="E4" s="0" t="n">
-        <f aca="false">D4+E3</f>
+      <c r="E4">
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5">
         <v>31</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5">
         <v>5</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <f aca="false">B5*C5</f>
+      <c r="D5">
+        <f t="shared" si="0"/>
         <v>155</v>
       </c>
-      <c r="E5" s="0" t="n">
-        <f aca="false">D5+E4</f>
+      <c r="E5">
+        <f t="shared" si="1"/>
         <v>455</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6">
         <v>30</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6">
         <v>6</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <f aca="false">B6*C6</f>
+      <c r="D6">
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
-      <c r="E6" s="0" t="n">
-        <f aca="false">D6+E5</f>
+      <c r="E6">
+        <f t="shared" si="1"/>
         <v>635</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7">
         <v>31</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7">
         <v>6</v>
       </c>
-      <c r="D7" s="0" t="n">
-        <f aca="false">B7*C7</f>
+      <c r="D7">
+        <f t="shared" si="0"/>
         <v>186</v>
       </c>
-      <c r="E7" s="0" t="n">
-        <f aca="false">D7+E6</f>
+      <c r="E7">
+        <f t="shared" si="1"/>
         <v>821</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8">
         <v>31</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8">
         <v>5</v>
       </c>
-      <c r="D8" s="0" t="n">
-        <f aca="false">B8*C8</f>
+      <c r="D8">
+        <f t="shared" si="0"/>
         <v>155</v>
       </c>
-      <c r="E8" s="0" t="n">
-        <f aca="false">D8+E7</f>
+      <c r="E8">
+        <f t="shared" si="1"/>
         <v>976</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9">
         <v>30</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9">
         <v>4</v>
       </c>
-      <c r="D9" s="0" t="n">
-        <f aca="false">B9*C9</f>
+      <c r="D9">
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="E9" s="0" t="n">
-        <f aca="false">D9+E8</f>
+      <c r="E9">
+        <f t="shared" si="1"/>
         <v>1096</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10">
         <v>31</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10">
         <v>3</v>
       </c>
-      <c r="D10" s="0" t="n">
-        <f aca="false">B10*C10</f>
+      <c r="D10">
+        <f t="shared" si="0"/>
         <v>93</v>
       </c>
-      <c r="E10" s="0" t="n">
-        <f aca="false">D10+E9</f>
+      <c r="E10">
+        <f t="shared" si="1"/>
         <v>1189</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11">
         <v>30</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11" s="0" t="n">
-        <f aca="false">B11*C11</f>
+      <c r="D11">
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="E11" s="0" t="n">
-        <f aca="false">D11+E10</f>
+      <c r="E11">
+        <f t="shared" si="1"/>
         <v>1249</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12">
         <v>31</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12" s="0" t="n">
-        <f aca="false">B12*C12</f>
+      <c r="D12">
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="E12" s="0" t="n">
-        <f aca="false">D12+E11</f>
+      <c r="E12">
+        <f t="shared" si="1"/>
         <v>1280</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScale="65" zoomScaleNormal="65" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScale="65" zoomScaleNormal="65" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add last couple of days of walks
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -68,7 +68,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -95,6 +95,11 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -217,7 +222,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -422,7 +427,7 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54.5</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v/>
@@ -467,11 +472,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="85480561"/>
-        <c:axId val="20701618"/>
+        <c:axId val="19828900"/>
+        <c:axId val="40596547"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85480561"/>
+        <c:axId val="19828900"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -507,14 +512,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20701618"/>
+        <c:crossAx val="40596547"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="20701618"/>
+        <c:axId val="40596547"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -560,7 +565,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85480561"/>
+        <c:crossAx val="19828900"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -608,9 +613,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>270720</xdr:colOff>
+      <xdr:colOff>270360</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>63000</xdr:rowOff>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -619,7 +624,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
-        <a:ext cx="9643320" cy="7111440"/>
+        <a:ext cx="9642960" cy="7111080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -667,7 +672,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -721,10 +726,10 @@
       </c>
       <c r="F2" s="0" t="n">
         <f aca="false">F1+G2</f>
-        <v>54.5</v>
+        <v>62</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>4.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add today's walk around Millwall
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -1,19 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Chart1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Chart1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,82 +24,53 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t xml:space="preserve">January</t>
+    <t>January</t>
   </si>
   <si>
-    <t xml:space="preserve">February</t>
+    <t>February</t>
   </si>
   <si>
-    <t xml:space="preserve">March</t>
+    <t>March</t>
   </si>
   <si>
-    <t xml:space="preserve">April</t>
+    <t>April</t>
   </si>
   <si>
-    <t xml:space="preserve">May</t>
+    <t>May</t>
   </si>
   <si>
-    <t xml:space="preserve">June</t>
+    <t>June</t>
   </si>
   <si>
-    <t xml:space="preserve">July</t>
+    <t>July</t>
   </si>
   <si>
-    <t xml:space="preserve">August</t>
+    <t>August</t>
   </si>
   <si>
-    <t xml:space="preserve">September</t>
+    <t>September</t>
   </si>
   <si>
-    <t xml:space="preserve">October</t>
+    <t>October</t>
   </si>
   <si>
-    <t xml:space="preserve">November</t>
+    <t>November</t>
   </si>
   <si>
-    <t xml:space="preserve">December</t>
+    <t>December</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -112,7 +82,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -120,45 +90,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -217,29 +159,44 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4a7ebb"/>
-            </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="4a7ebb"/>
+                <a:srgbClr val="4A7EBB"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -254,6 +211,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -351,12 +309,9 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="be4b48"/>
-            </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="be4b48"/>
+                <a:srgbClr val="BE4B48"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -371,6 +326,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -427,43 +383,21 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v/>
+                  <c:v>66</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
             <a:ln>
@@ -471,12 +405,13 @@
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="19828900"/>
-        <c:axId val="40596547"/>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="84132224"/>
+        <c:axId val="84133760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="19828900"/>
+        <c:axId val="84132224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -496,30 +431,33 @@
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:uFill>
                   <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a:uFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40596547"/>
+        <c:crossAx val="84133760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40596547"/>
+        <c:axId val="84133760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -549,29 +487,31 @@
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:uFill>
                   <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a:uFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19828900"/>
+        <c:crossAx val="84132224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -590,20 +530,26 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln>
       <a:noFill/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -617,14 +563,14 @@
       <xdr:row>37</xdr:row>
       <xdr:rowOff>62640</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
-        <a:ext cx="9642960" cy="7111080"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -637,350 +583,602 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="true"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+    <sheetView topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="n">
+      <c r="B1">
         <v>31</v>
       </c>
-      <c r="C1" s="0" t="n">
+      <c r="C1">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="n">
-        <f aca="false">B1*C1</f>
+      <c r="D1">
+        <f t="shared" ref="D1:D12" si="0">B1*C1</f>
         <v>31</v>
       </c>
-      <c r="E1" s="0" t="n">
-        <f aca="false">D1</f>
+      <c r="E1">
+        <f>D1</f>
         <v>31</v>
       </c>
-      <c r="F1" s="0" t="n">
-        <f aca="false">G1</f>
+      <c r="F1">
+        <f>G1</f>
         <v>50</v>
       </c>
-      <c r="G1" s="0" t="n">
+      <c r="G1">
         <v>50</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2">
         <v>28</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2">
         <v>2</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <f aca="false">B2*C2</f>
+      <c r="D2">
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <f aca="false">D2+E1</f>
+      <c r="E2">
+        <f t="shared" ref="E2:E12" si="1">D2+E1</f>
         <v>87</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <f aca="false">F1+G2</f>
-        <v>62</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>12</v>
+      <c r="F2">
+        <f>F1+G2</f>
+        <v>66</v>
+      </c>
+      <c r="G2">
+        <v>16</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3">
         <v>31</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3">
         <v>3</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <f aca="false">B3*C3</f>
+      <c r="D3">
+        <f t="shared" si="0"/>
         <v>93</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <f aca="false">D3+E2</f>
+      <c r="E3">
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4">
         <v>30</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4">
         <v>4</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <f aca="false">B4*C4</f>
+      <c r="D4">
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="E4" s="0" t="n">
-        <f aca="false">D4+E3</f>
+      <c r="E4">
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5">
         <v>31</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5">
         <v>5</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <f aca="false">B5*C5</f>
+      <c r="D5">
+        <f t="shared" si="0"/>
         <v>155</v>
       </c>
-      <c r="E5" s="0" t="n">
-        <f aca="false">D5+E4</f>
+      <c r="E5">
+        <f t="shared" si="1"/>
         <v>455</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6">
         <v>30</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6">
         <v>6</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <f aca="false">B6*C6</f>
+      <c r="D6">
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
-      <c r="E6" s="0" t="n">
-        <f aca="false">D6+E5</f>
+      <c r="E6">
+        <f t="shared" si="1"/>
         <v>635</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7">
         <v>31</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7">
         <v>6</v>
       </c>
-      <c r="D7" s="0" t="n">
-        <f aca="false">B7*C7</f>
+      <c r="D7">
+        <f t="shared" si="0"/>
         <v>186</v>
       </c>
-      <c r="E7" s="0" t="n">
-        <f aca="false">D7+E6</f>
+      <c r="E7">
+        <f t="shared" si="1"/>
         <v>821</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8">
         <v>31</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8">
         <v>5</v>
       </c>
-      <c r="D8" s="0" t="n">
-        <f aca="false">B8*C8</f>
+      <c r="D8">
+        <f t="shared" si="0"/>
         <v>155</v>
       </c>
-      <c r="E8" s="0" t="n">
-        <f aca="false">D8+E7</f>
+      <c r="E8">
+        <f t="shared" si="1"/>
         <v>976</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9">
         <v>30</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9">
         <v>4</v>
       </c>
-      <c r="D9" s="0" t="n">
-        <f aca="false">B9*C9</f>
+      <c r="D9">
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="E9" s="0" t="n">
-        <f aca="false">D9+E8</f>
+      <c r="E9">
+        <f t="shared" si="1"/>
         <v>1096</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10">
         <v>31</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10">
         <v>3</v>
       </c>
-      <c r="D10" s="0" t="n">
-        <f aca="false">B10*C10</f>
+      <c r="D10">
+        <f t="shared" si="0"/>
         <v>93</v>
       </c>
-      <c r="E10" s="0" t="n">
-        <f aca="false">D10+E9</f>
+      <c r="E10">
+        <f t="shared" si="1"/>
         <v>1189</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11">
         <v>30</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11" s="0" t="n">
-        <f aca="false">B11*C11</f>
+      <c r="D11">
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="E11" s="0" t="n">
-        <f aca="false">D11+E10</f>
+      <c r="E11">
+        <f t="shared" si="1"/>
         <v>1249</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12">
         <v>31</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12" s="0" t="n">
-        <f aca="false">B12*C12</f>
+      <c r="D12">
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="E12" s="0" t="n">
-        <f aca="false">D12+E11</f>
+      <c r="E12">
+        <f t="shared" si="1"/>
         <v>1280</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add walk to OA!
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -383,7 +383,7 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>66</c:v>
+                  <c:v>67.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -407,11 +407,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="84132224"/>
-        <c:axId val="84133760"/>
+        <c:axId val="73401856"/>
+        <c:axId val="73403392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84132224"/>
+        <c:axId val="73401856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -449,7 +449,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84133760"/>
+        <c:crossAx val="73403392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -457,7 +457,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84133760"/>
+        <c:axId val="73403392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -505,7 +505,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84132224"/>
+        <c:crossAx val="73401856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -949,10 +949,10 @@
       </c>
       <c r="F2">
         <f>F1+G2</f>
-        <v>66</v>
+        <v>67.5</v>
       </c>
       <c r="G2">
-        <v>16</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add this morning's walk
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27211"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marks/projects/walk/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="987"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="1" r:id="rId1"/>
@@ -12,8 +17,14 @@
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -205,6 +216,13 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -213,6 +231,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -265,40 +288,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>31</c:v>
+                  <c:v>31.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>87</c:v>
+                  <c:v>87.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>180</c:v>
+                  <c:v>180.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>300</c:v>
+                  <c:v>300.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>455</c:v>
+                  <c:v>455.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>635</c:v>
+                  <c:v>635.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>821</c:v>
+                  <c:v>821.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>976</c:v>
+                  <c:v>976.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1096</c:v>
+                  <c:v>1096.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1189</c:v>
+                  <c:v>1189.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1249</c:v>
+                  <c:v>1249.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1280</c:v>
+                  <c:v>1280.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -320,6 +343,13 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -328,6 +358,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -380,10 +415,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>67.5</c:v>
+                  <c:v>68.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -405,13 +440,12 @@
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="73401856"/>
-        <c:axId val="73403392"/>
+        <c:axId val="-2082553488"/>
+        <c:axId val="-2082550272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="73401856"/>
+        <c:axId val="-2082553488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -449,7 +483,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73403392"/>
+        <c:crossAx val="-2082550272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -457,7 +491,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73403392"/>
+        <c:axId val="-2082550272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -505,7 +539,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73401856"/>
+        <c:crossAx val="-2082553488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -520,6 +554,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -626,12 +661,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -661,12 +696,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -870,19 +905,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1025" width="8.7109375"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -894,16 +926,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1025" width="8.7109375"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -929,7 +958,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -949,13 +978,13 @@
       </c>
       <c r="F2">
         <f>F1+G2</f>
-        <v>67.5</v>
+        <v>68.5</v>
       </c>
       <c r="G2">
-        <v>17.5</v>
+        <v>18.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -974,7 +1003,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -993,7 +1022,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1012,7 +1041,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1031,7 +1060,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1050,7 +1079,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1069,7 +1098,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1088,7 +1117,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1107,7 +1136,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1126,7 +1155,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1155,12 +1184,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1025" width="8.7109375"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1171,12 +1197,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1025" width="8.7109375"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Add just one mile today
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="1" state="visible" r:id="rId2"/>
@@ -68,7 +68,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -95,6 +95,11 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -422,7 +427,7 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>73.9</c:v>
+                  <c:v>74.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v/>
@@ -467,11 +472,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="52982711"/>
-        <c:axId val="63742627"/>
+        <c:axId val="30185847"/>
+        <c:axId val="54880517"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="52982711"/>
+        <c:axId val="30185847"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -507,14 +512,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63742627"/>
+        <c:crossAx val="54880517"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63742627"/>
+        <c:axId val="54880517"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -560,7 +565,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52982711"/>
+        <c:crossAx val="30185847"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -608,9 +613,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>270000</xdr:colOff>
+      <xdr:colOff>269640</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>62280</xdr:rowOff>
+      <xdr:rowOff>61920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -619,7 +624,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
-        <a:ext cx="9756720" cy="7110720"/>
+        <a:ext cx="9756360" cy="7110360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -639,7 +644,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -666,7 +671,7 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -721,10 +726,10 @@
       </c>
       <c r="F2" s="0" t="n">
         <f aca="false">F1+G2</f>
-        <v>73.9</v>
+        <v>74.9</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>23.9</v>
+        <v>24.9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add walk to Westfield
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -383,7 +383,7 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>82.4</c:v>
+                  <c:v>85.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -407,11 +407,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="74128000"/>
-        <c:axId val="74135808"/>
+        <c:axId val="42222720"/>
+        <c:axId val="42224256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74128000"/>
+        <c:axId val="42222720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -449,7 +449,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74135808"/>
+        <c:crossAx val="42224256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -457,7 +457,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74135808"/>
+        <c:axId val="42224256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -505,7 +505,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74128000"/>
+        <c:crossAx val="42222720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -896,7 +896,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,10 +950,10 @@
       </c>
       <c r="F2">
         <f>F1+G2</f>
-        <v>82.4</v>
+        <v>85.9</v>
       </c>
       <c r="G2">
-        <v>32.4</v>
+        <v>35.9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add last two days' feeble efforts
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="1" state="visible" r:id="rId2"/>
@@ -427,7 +427,7 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>88.4</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v/>
@@ -472,11 +472,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="20198124"/>
-        <c:axId val="80782456"/>
+        <c:axId val="53991534"/>
+        <c:axId val="88476396"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="20198124"/>
+        <c:axId val="53991534"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -512,14 +512,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80782456"/>
+        <c:crossAx val="88476396"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80782456"/>
+        <c:axId val="88476396"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -565,7 +565,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20198124"/>
+        <c:crossAx val="53991534"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -613,9 +613,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>268920</xdr:colOff>
+      <xdr:colOff>268560</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>61200</xdr:rowOff>
+      <xdr:rowOff>60840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -624,7 +624,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
-        <a:ext cx="9755640" cy="7109640"/>
+        <a:ext cx="9755280" cy="7109280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -644,7 +644,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D39" activeCellId="0" sqref="D39"/>
     </sheetView>
   </sheetViews>
@@ -671,7 +671,7 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -726,10 +726,10 @@
       </c>
       <c r="F2" s="0" t="n">
         <f aca="false">F1+G2</f>
-        <v>88.4</v>
+        <v>92</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>38.4</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Make the total right according to the text files
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -427,7 +427,7 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>92</c:v>
+                  <c:v>92.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v/>
@@ -472,11 +472,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="53991534"/>
-        <c:axId val="88476396"/>
+        <c:axId val="39132230"/>
+        <c:axId val="14008835"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="53991534"/>
+        <c:axId val="39132230"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -512,14 +512,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88476396"/>
+        <c:crossAx val="14008835"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88476396"/>
+        <c:axId val="14008835"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -565,7 +565,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53991534"/>
+        <c:crossAx val="39132230"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -613,9 +613,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+      <xdr:colOff>268200</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>60840</xdr:rowOff>
+      <xdr:rowOff>60480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -624,7 +624,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
-        <a:ext cx="9755280" cy="7109280"/>
+        <a:ext cx="9754920" cy="7108920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -726,10 +726,10 @@
       </c>
       <c r="F2" s="0" t="n">
         <f aca="false">F1+G2</f>
-        <v>92</v>
+        <v>92.4</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>42</v>
+        <v>42.4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add isle of dogs
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -1,19 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Chart1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Chart1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,82 +24,53 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t xml:space="preserve">January</t>
+    <t>January</t>
   </si>
   <si>
-    <t xml:space="preserve">February</t>
+    <t>February</t>
   </si>
   <si>
-    <t xml:space="preserve">March</t>
+    <t>March</t>
   </si>
   <si>
-    <t xml:space="preserve">April</t>
+    <t>April</t>
   </si>
   <si>
-    <t xml:space="preserve">May</t>
+    <t>May</t>
   </si>
   <si>
-    <t xml:space="preserve">June</t>
+    <t>June</t>
   </si>
   <si>
-    <t xml:space="preserve">July</t>
+    <t>July</t>
   </si>
   <si>
-    <t xml:space="preserve">August</t>
+    <t>August</t>
   </si>
   <si>
-    <t xml:space="preserve">September</t>
+    <t>September</t>
   </si>
   <si>
-    <t xml:space="preserve">October</t>
+    <t>October</t>
   </si>
   <si>
-    <t xml:space="preserve">November</t>
+    <t>November</t>
   </si>
   <si>
-    <t xml:space="preserve">December</t>
+    <t>December</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -112,7 +82,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -120,45 +90,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -217,29 +159,44 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4a7ebb"/>
-            </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="4a7ebb"/>
+                <a:srgbClr val="4A7EBB"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -254,6 +211,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -351,12 +309,9 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="be4b48"/>
-            </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="be4b48"/>
+                <a:srgbClr val="BE4B48"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -371,6 +326,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
@@ -427,43 +383,21 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>92.4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v/>
+                  <c:v>97.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
             <a:ln>
@@ -471,12 +405,13 @@
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="39132230"/>
-        <c:axId val="14008835"/>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="40057472"/>
+        <c:axId val="40065280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39132230"/>
+        <c:axId val="40057472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -496,30 +431,33 @@
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:uFill>
                   <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a:uFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14008835"/>
+        <c:crossAx val="40065280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="14008835"/>
+        <c:axId val="40065280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -549,29 +487,31 @@
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:uFill>
                   <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a:uFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39132230"/>
+        <c:crossAx val="40057472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -580,6 +520,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -590,20 +531,26 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln>
       <a:noFill/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -617,14 +564,14 @@
       <xdr:row>37</xdr:row>
       <xdr:rowOff>60480</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
-        <a:ext cx="9754920" cy="7108920"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -637,350 +584,602 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="true"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D39" activeCellId="0" sqref="D39"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.89068825910931"/>
+    <col min="1" max="1025" width="8.85546875"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.89068825910931"/>
+    <col min="1" max="1025" width="8.85546875"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="n">
+      <c r="B1">
         <v>31</v>
       </c>
-      <c r="C1" s="0" t="n">
+      <c r="C1">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="n">
-        <f aca="false">B1*C1</f>
+      <c r="D1">
+        <f t="shared" ref="D1:D12" si="0">B1*C1</f>
         <v>31</v>
       </c>
-      <c r="E1" s="0" t="n">
-        <f aca="false">D1</f>
+      <c r="E1">
+        <f>D1</f>
         <v>31</v>
       </c>
-      <c r="F1" s="0" t="n">
-        <f aca="false">G1</f>
+      <c r="F1">
+        <f>G1</f>
         <v>50</v>
       </c>
-      <c r="G1" s="0" t="n">
+      <c r="G1">
         <v>50</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2">
         <v>28</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2">
         <v>2</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <f aca="false">B2*C2</f>
+      <c r="D2">
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <f aca="false">D2+E1</f>
+      <c r="E2">
+        <f t="shared" ref="E2:E12" si="1">D2+E1</f>
         <v>87</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <f aca="false">F1+G2</f>
-        <v>92.4</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>42.4</v>
+      <c r="F2">
+        <f>F1+G2</f>
+        <v>97.4</v>
+      </c>
+      <c r="G2">
+        <v>47.4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3">
         <v>31</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3">
         <v>3</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <f aca="false">B3*C3</f>
+      <c r="D3">
+        <f t="shared" si="0"/>
         <v>93</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <f aca="false">D3+E2</f>
+      <c r="E3">
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4">
         <v>30</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4">
         <v>4</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <f aca="false">B4*C4</f>
+      <c r="D4">
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="E4" s="0" t="n">
-        <f aca="false">D4+E3</f>
+      <c r="E4">
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5">
         <v>31</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5">
         <v>5</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <f aca="false">B5*C5</f>
+      <c r="D5">
+        <f t="shared" si="0"/>
         <v>155</v>
       </c>
-      <c r="E5" s="0" t="n">
-        <f aca="false">D5+E4</f>
+      <c r="E5">
+        <f t="shared" si="1"/>
         <v>455</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6">
         <v>30</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6">
         <v>6</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <f aca="false">B6*C6</f>
+      <c r="D6">
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
-      <c r="E6" s="0" t="n">
-        <f aca="false">D6+E5</f>
+      <c r="E6">
+        <f t="shared" si="1"/>
         <v>635</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7">
         <v>31</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7">
         <v>6</v>
       </c>
-      <c r="D7" s="0" t="n">
-        <f aca="false">B7*C7</f>
+      <c r="D7">
+        <f t="shared" si="0"/>
         <v>186</v>
       </c>
-      <c r="E7" s="0" t="n">
-        <f aca="false">D7+E6</f>
+      <c r="E7">
+        <f t="shared" si="1"/>
         <v>821</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8">
         <v>31</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8">
         <v>5</v>
       </c>
-      <c r="D8" s="0" t="n">
-        <f aca="false">B8*C8</f>
+      <c r="D8">
+        <f t="shared" si="0"/>
         <v>155</v>
       </c>
-      <c r="E8" s="0" t="n">
-        <f aca="false">D8+E7</f>
+      <c r="E8">
+        <f t="shared" si="1"/>
         <v>976</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9">
         <v>30</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9">
         <v>4</v>
       </c>
-      <c r="D9" s="0" t="n">
-        <f aca="false">B9*C9</f>
+      <c r="D9">
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="E9" s="0" t="n">
-        <f aca="false">D9+E8</f>
+      <c r="E9">
+        <f t="shared" si="1"/>
         <v>1096</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10">
         <v>31</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10">
         <v>3</v>
       </c>
-      <c r="D10" s="0" t="n">
-        <f aca="false">B10*C10</f>
+      <c r="D10">
+        <f t="shared" si="0"/>
         <v>93</v>
       </c>
-      <c r="E10" s="0" t="n">
-        <f aca="false">D10+E9</f>
+      <c r="E10">
+        <f t="shared" si="1"/>
         <v>1189</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11">
         <v>30</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11" s="0" t="n">
-        <f aca="false">B11*C11</f>
+      <c r="D11">
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="E11" s="0" t="n">
-        <f aca="false">D11+E10</f>
+      <c r="E11">
+        <f t="shared" si="1"/>
         <v>1249</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12">
         <v>31</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12" s="0" t="n">
-        <f aca="false">B12*C12</f>
+      <c r="D12">
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="E12" s="0" t="n">
-        <f aca="false">D12+E11</f>
+      <c r="E12">
+        <f t="shared" si="1"/>
         <v>1280</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.89068825910931"/>
+    <col min="1" max="1025" width="8.85546875"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.89068825910931"/>
+    <col min="1" max="1025" width="8.85546875"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add walk to Ickenham and Canary Wharf
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -383,7 +383,7 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>97.4</c:v>
+                  <c:v>101.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -407,11 +407,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="40057472"/>
-        <c:axId val="40065280"/>
+        <c:axId val="80419456"/>
+        <c:axId val="80427264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40057472"/>
+        <c:axId val="80419456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -449,7 +449,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40065280"/>
+        <c:crossAx val="80427264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -457,7 +457,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40065280"/>
+        <c:axId val="80427264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -505,7 +505,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40057472"/>
+        <c:crossAx val="80419456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -896,7 +896,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,10 +950,10 @@
       </c>
       <c r="F2">
         <f>F1+G2</f>
-        <v>97.4</v>
+        <v>101.9</v>
       </c>
       <c r="G2">
-        <v>47.4</v>
+        <v>51.9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add today's walk in Athens
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="987" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="1" r:id="rId1"/>
@@ -383,7 +383,7 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>101.9</c:v>
+                  <c:v>104.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -407,11 +407,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="80419456"/>
-        <c:axId val="80427264"/>
+        <c:axId val="67417984"/>
+        <c:axId val="67419520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80419456"/>
+        <c:axId val="67417984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -449,7 +449,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80427264"/>
+        <c:crossAx val="67419520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -457,7 +457,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80427264"/>
+        <c:axId val="67419520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -505,7 +505,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80419456"/>
+        <c:crossAx val="67417984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -520,7 +520,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -896,7 +895,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,10 +949,10 @@
       </c>
       <c r="F2">
         <f>F1+G2</f>
-        <v>101.9</v>
+        <v>104.3</v>
       </c>
       <c r="G2">
-        <v>51.9</v>
+        <v>54.3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add another walk to the platia
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="987" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="987"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="1" r:id="rId1"/>
@@ -383,7 +383,7 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>104.3</c:v>
+                  <c:v>106.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -407,11 +407,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="67417984"/>
-        <c:axId val="67419520"/>
+        <c:axId val="68665728"/>
+        <c:axId val="68667264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="67417984"/>
+        <c:axId val="68665728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -449,7 +449,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67419520"/>
+        <c:crossAx val="68667264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -457,7 +457,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67419520"/>
+        <c:axId val="68667264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -505,7 +505,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67417984"/>
+        <c:crossAx val="68665728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -520,6 +520,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -875,7 +876,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
@@ -894,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,10 +950,10 @@
       </c>
       <c r="F2">
         <f>F1+G2</f>
-        <v>104.3</v>
+        <v>106.9</v>
       </c>
       <c r="G2">
-        <v>54.3</v>
+        <v>56.9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add today's walk around Athens
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -383,7 +383,7 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>106.9</c:v>
+                  <c:v>109.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -407,11 +407,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="68665728"/>
-        <c:axId val="68667264"/>
+        <c:axId val="69266432"/>
+        <c:axId val="70062848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="68665728"/>
+        <c:axId val="69266432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -449,7 +449,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68667264"/>
+        <c:crossAx val="70062848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -457,7 +457,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68667264"/>
+        <c:axId val="70062848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -505,7 +505,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68665728"/>
+        <c:crossAx val="69266432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -950,10 +950,10 @@
       </c>
       <c r="F2">
         <f>F1+G2</f>
-        <v>106.9</v>
+        <v>109.2</v>
       </c>
       <c r="G2">
-        <v>56.9</v>
+        <v>59.2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add walk to the platia and back@
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="987"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="987" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="1" r:id="rId1"/>
@@ -383,7 +383,7 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>109.2</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -407,11 +407,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="69266432"/>
-        <c:axId val="70062848"/>
+        <c:axId val="68130688"/>
+        <c:axId val="68132224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69266432"/>
+        <c:axId val="68130688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -449,7 +449,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70062848"/>
+        <c:crossAx val="68132224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -457,7 +457,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70062848"/>
+        <c:axId val="68132224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -505,7 +505,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69266432"/>
+        <c:crossAx val="68130688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -876,7 +876,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
@@ -895,7 +895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -950,10 +950,10 @@
       </c>
       <c r="F2">
         <f>F1+G2</f>
-        <v>109.2</v>
+        <v>112</v>
       </c>
       <c r="G2">
-        <v>59.2</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add today's walk to the platia
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="987" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="987"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="1" r:id="rId1"/>
@@ -383,7 +383,7 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>112</c:v>
+                  <c:v>114.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -407,11 +407,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="68130688"/>
-        <c:axId val="68132224"/>
+        <c:axId val="68866432"/>
+        <c:axId val="68867968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="68130688"/>
+        <c:axId val="68866432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -449,7 +449,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68132224"/>
+        <c:crossAx val="68867968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -457,7 +457,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68132224"/>
+        <c:axId val="68867968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -505,7 +505,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68130688"/>
+        <c:crossAx val="68866432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -876,7 +876,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
@@ -895,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,10 +950,10 @@
       </c>
       <c r="F2">
         <f>F1+G2</f>
-        <v>112</v>
+        <v>114.5</v>
       </c>
       <c r="G2">
-        <v>62</v>
+        <v>64.5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Change the spreadsheet a bit
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>January</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>December</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -193,6 +199,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Target</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28440">
               <a:solidFill>
@@ -216,7 +225,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$1:$A$12</c:f>
+              <c:f>Sheet1!$A$2:$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -260,7 +269,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$1:$E$12</c:f>
+              <c:f>Sheet1!$E$2:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -308,6 +317,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Actual</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28440">
               <a:solidFill>
@@ -331,7 +343,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$1:$A$12</c:f>
+              <c:f>Sheet1!$A$2:$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -375,7 +387,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$1:$F$12</c:f>
+              <c:f>Sheet1!$F$2:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -407,11 +419,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="68866432"/>
-        <c:axId val="68867968"/>
+        <c:axId val="57644928"/>
+        <c:axId val="57646464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="68866432"/>
+        <c:axId val="57644928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -449,7 +461,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68867968"/>
+        <c:crossAx val="57646464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -457,7 +469,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68867968"/>
+        <c:axId val="57646464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -505,7 +517,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68866432"/>
+        <c:crossAx val="57644928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -876,8 +888,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,10 +905,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,243 +917,251 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>31</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <f t="shared" ref="D1:D12" si="0">B1*C1</f>
-        <v>31</v>
-      </c>
-      <c r="E1">
-        <f>D1</f>
-        <v>31</v>
-      </c>
-      <c r="F1">
-        <f>G1</f>
-        <v>50</v>
-      </c>
-      <c r="G1">
-        <v>50</v>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>31</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>28</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
       <c r="D2">
-        <f t="shared" si="0"/>
-        <v>56</v>
+        <f t="shared" ref="D2:D13" si="0">B2*C2</f>
+        <v>31</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E12" si="1">D2+E1</f>
-        <v>87</v>
+        <f>D2</f>
+        <v>31</v>
       </c>
       <c r="F2">
-        <f>F1+G2</f>
-        <v>114.5</v>
+        <f>G2</f>
+        <v>50</v>
       </c>
       <c r="G2">
-        <v>64.5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>28</v>
+      </c>
+      <c r="C3">
         <v>2</v>
-      </c>
-      <c r="B3">
-        <v>31</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="E3">
-        <f t="shared" si="1"/>
-        <v>180</v>
+        <f t="shared" ref="E3:E13" si="1">D3+E2</f>
+        <v>87</v>
+      </c>
+      <c r="F3">
+        <f>F2+G3</f>
+        <v>114.5</v>
+      </c>
+      <c r="G3">
+        <v>64.5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>31</v>
+      </c>
+      <c r="C4">
         <v>3</v>
-      </c>
-      <c r="B4">
-        <v>30</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>300</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>30</v>
+      </c>
+      <c r="C5">
         <v>4</v>
-      </c>
-      <c r="B5">
-        <v>31</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>455</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>31</v>
+      </c>
+      <c r="C6">
         <v>5</v>
-      </c>
-      <c r="B6">
-        <v>30</v>
-      </c>
-      <c r="C6">
-        <v>6</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>635</v>
+        <v>455</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>821</v>
+        <v>635</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>31</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>155</v>
+        <v>186</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>976</v>
+        <v>821</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>1096</v>
+        <v>976</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>1189</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>1249</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
         <v>31</v>
       </c>
-      <c r="E12">
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="E13">
         <f t="shared" si="1"/>
         <v>1280</v>
       </c>

</xml_diff>

<commit_message>
Add a walk with the dog
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="987"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="987" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="1" r:id="rId1"/>
@@ -395,7 +395,7 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>114.5</c:v>
+                  <c:v>116.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -419,11 +419,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="57644928"/>
-        <c:axId val="57646464"/>
+        <c:axId val="73701248"/>
+        <c:axId val="73702784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="57644928"/>
+        <c:axId val="73701248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -461,7 +461,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57646464"/>
+        <c:crossAx val="73702784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -469,7 +469,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57646464"/>
+        <c:axId val="73702784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -517,7 +517,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57644928"/>
+        <c:crossAx val="73701248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -888,7 +888,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A23" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
@@ -907,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,10 +970,10 @@
       </c>
       <c r="F3">
         <f>F2+G3</f>
-        <v>114.5</v>
+        <v>116.8</v>
       </c>
       <c r="G3">
-        <v>64.5</v>
+        <v>66.8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Walk to Miki Theodorakis park and back
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="987"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>January</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>December</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -193,6 +199,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Target</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28440">
               <a:solidFill>
@@ -216,7 +225,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$1:$A$12</c:f>
+              <c:f>Sheet1!$A$2:$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -260,7 +269,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$1:$E$12</c:f>
+              <c:f>Sheet1!$E$2:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -308,6 +317,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Actual</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28440">
               <a:solidFill>
@@ -331,7 +343,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$1:$A$12</c:f>
+              <c:f>Sheet1!$A$2:$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -375,7 +387,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$1:$F$12</c:f>
+              <c:f>Sheet1!$F$2:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -383,7 +395,7 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>101.9</c:v>
+                  <c:v>118.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -407,11 +419,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="80419456"/>
-        <c:axId val="80427264"/>
+        <c:axId val="83219200"/>
+        <c:axId val="83220736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80419456"/>
+        <c:axId val="83219200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -449,7 +461,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80427264"/>
+        <c:crossAx val="83220736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -457,7 +469,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80427264"/>
+        <c:axId val="83220736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -505,7 +517,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80419456"/>
+        <c:crossAx val="83219200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -876,8 +888,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,10 +905,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,243 +917,251 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>31</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <f t="shared" ref="D1:D12" si="0">B1*C1</f>
-        <v>31</v>
-      </c>
-      <c r="E1">
-        <f>D1</f>
-        <v>31</v>
-      </c>
-      <c r="F1">
-        <f>G1</f>
-        <v>50</v>
-      </c>
-      <c r="G1">
-        <v>50</v>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>31</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>28</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
       <c r="D2">
-        <f t="shared" si="0"/>
-        <v>56</v>
+        <f t="shared" ref="D2:D13" si="0">B2*C2</f>
+        <v>31</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E12" si="1">D2+E1</f>
-        <v>87</v>
+        <f>D2</f>
+        <v>31</v>
       </c>
       <c r="F2">
-        <f>F1+G2</f>
-        <v>101.9</v>
+        <f>G2</f>
+        <v>50</v>
       </c>
       <c r="G2">
-        <v>51.9</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>28</v>
+      </c>
+      <c r="C3">
         <v>2</v>
-      </c>
-      <c r="B3">
-        <v>31</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="E3">
-        <f t="shared" si="1"/>
-        <v>180</v>
+        <f t="shared" ref="E3:E13" si="1">D3+E2</f>
+        <v>87</v>
+      </c>
+      <c r="F3">
+        <f>F2+G3</f>
+        <v>118.6</v>
+      </c>
+      <c r="G3">
+        <v>68.599999999999994</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>31</v>
+      </c>
+      <c r="C4">
         <v>3</v>
-      </c>
-      <c r="B4">
-        <v>30</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>300</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>30</v>
+      </c>
+      <c r="C5">
         <v>4</v>
-      </c>
-      <c r="B5">
-        <v>31</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>455</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>31</v>
+      </c>
+      <c r="C6">
         <v>5</v>
-      </c>
-      <c r="B6">
-        <v>30</v>
-      </c>
-      <c r="C6">
-        <v>6</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>635</v>
+        <v>455</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>821</v>
+        <v>635</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>31</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>155</v>
+        <v>186</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>976</v>
+        <v>821</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>1096</v>
+        <v>976</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>1189</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>1249</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
         <v>31</v>
       </c>
-      <c r="E12">
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="E13">
         <f t="shared" si="1"/>
         <v>1280</v>
       </c>

</xml_diff>

<commit_message>
Add yesterday's delicious walk through Pendelis
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -395,7 +395,7 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>118.6</c:v>
+                  <c:v>121.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -419,11 +419,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="83219200"/>
-        <c:axId val="83220736"/>
+        <c:axId val="86131840"/>
+        <c:axId val="86133376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83219200"/>
+        <c:axId val="86131840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -461,7 +461,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83220736"/>
+        <c:crossAx val="86133376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -469,7 +469,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83220736"/>
+        <c:axId val="86133376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -517,7 +517,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83219200"/>
+        <c:crossAx val="86131840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -888,7 +888,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
@@ -908,7 +908,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,10 +970,10 @@
       </c>
       <c r="F3">
         <f>F2+G3</f>
-        <v>118.6</v>
+        <v>121.6</v>
       </c>
       <c r="G3">
-        <v>68.599999999999994</v>
+        <v>71.599999999999994</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add walk around Millwall docks
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -395,7 +395,7 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>121.6</c:v>
+                  <c:v>126.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -419,11 +419,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="86131840"/>
-        <c:axId val="86133376"/>
+        <c:axId val="84412672"/>
+        <c:axId val="84434944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="86131840"/>
+        <c:axId val="84412672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -461,7 +461,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86133376"/>
+        <c:crossAx val="84434944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -469,7 +469,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86133376"/>
+        <c:axId val="84434944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -517,7 +517,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86131840"/>
+        <c:crossAx val="84412672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -908,7 +908,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,10 +970,10 @@
       </c>
       <c r="F3">
         <f>F2+G3</f>
-        <v>121.6</v>
+        <v>126.1</v>
       </c>
       <c r="G3">
-        <v>71.599999999999994</v>
+        <v>76.099999999999994</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add the walk back from Uxbridge to Ickenham
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27211"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marks/projects/walk/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="987"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="15480" tabRatio="987"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="1" r:id="rId1"/>
@@ -17,11 +12,8 @@
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="145621" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -297,40 +289,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>31.0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>87.0</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>180.0</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>300.0</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>455.0</c:v>
+                  <c:v>455</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>635.0</c:v>
+                  <c:v>635</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>821.0</c:v>
+                  <c:v>821</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>976.0</c:v>
+                  <c:v>976</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1096.0</c:v>
+                  <c:v>1096</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1189.0</c:v>
+                  <c:v>1189</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1249.0</c:v>
+                  <c:v>1249</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1280.0</c:v>
+                  <c:v>1280</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -427,10 +419,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>127.1</c:v>
+                  <c:v>122.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -452,12 +444,13 @@
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2145815344"/>
-        <c:axId val="2145818144"/>
+        <c:axId val="93591808"/>
+        <c:axId val="93614080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2145815344"/>
+        <c:axId val="93591808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -495,7 +488,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2145818144"/>
+        <c:crossAx val="93614080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -503,7 +496,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2145818144"/>
+        <c:axId val="93614080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -551,7 +544,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2145815344"/>
+        <c:crossAx val="93591808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -926,7 +919,7 @@
       <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -939,12 +932,12 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
         <v>12</v>
       </c>
@@ -952,7 +945,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -978,7 +971,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -998,13 +991,13 @@
       </c>
       <c r="F3">
         <f>F2+G3</f>
-        <v>127.1</v>
+        <v>122.1</v>
       </c>
       <c r="G3">
-        <v>77.099999999999994</v>
+        <v>72.099999999999994</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1023,7 +1016,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1042,7 +1035,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1061,7 +1054,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1080,7 +1073,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1099,7 +1092,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1118,7 +1111,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1137,7 +1130,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1156,7 +1149,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1175,7 +1168,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1206,7 +1199,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1219,7 +1212,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Make the sort script generate a csv essentially
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="987"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" tabRatio="987" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="1" r:id="rId1"/>
@@ -430,7 +430,7 @@
                   <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>127.1</c:v>
+                  <c:v>118.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -453,11 +453,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="2145815344"/>
-        <c:axId val="2145818144"/>
+        <c:axId val="2101363488"/>
+        <c:axId val="2101360256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2145815344"/>
+        <c:axId val="2101363488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -495,7 +495,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2145818144"/>
+        <c:crossAx val="2101360256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -503,7 +503,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2145818144"/>
+        <c:axId val="2101360256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -551,7 +551,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2145815344"/>
+        <c:crossAx val="2101363488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -922,7 +922,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
@@ -938,7 +938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -998,10 +998,10 @@
       </c>
       <c r="F3">
         <f>F2+G3</f>
-        <v>127.1</v>
+        <v>118.6</v>
       </c>
       <c r="G3">
-        <v>77.099999999999994</v>
+        <v>68.599999999999994</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add the walk around Uxbridge@
</commit_message>
<xml_diff>
--- a/WalkChart.xlsx
+++ b/WalkChart.xlsx
@@ -430,7 +430,7 @@
                   <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>122.1</c:v>
+                  <c:v>123.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -453,11 +453,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="-2110148368"/>
-        <c:axId val="-2133273680"/>
+        <c:axId val="2130065248"/>
+        <c:axId val="2127163152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2110148368"/>
+        <c:axId val="2130065248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -495,7 +495,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133273680"/>
+        <c:crossAx val="2127163152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -503,7 +503,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133273680"/>
+        <c:axId val="2127163152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -551,7 +551,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2110148368"/>
+        <c:crossAx val="2130065248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -566,7 +566,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -939,7 +938,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -998,10 +997,10 @@
       </c>
       <c r="F3">
         <f>F2+G3</f>
-        <v>122.1</v>
+        <v>123.6</v>
       </c>
       <c r="G3">
-        <v>72.099999999999994</v>
+        <v>73.599999999999994</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>